<commit_message>
Adding Test Cases With More Data to Validate
</commit_message>
<xml_diff>
--- a/Numadic1/Data/projecttestcase.xlsx
+++ b/Numadic1/Data/projecttestcase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>SI No</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>https://linkedin.com/in/shaibaz</t>
+  </si>
+  <si>
+    <t>9900333333</t>
+  </si>
+  <si>
+    <t>560002</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
 </sst>
 </file>
@@ -717,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,8 +812,8 @@
       <c r="C2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D2">
-        <v>9900333333</v>
+      <c r="D2" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E2" t="s">
         <v>38</v>
@@ -812,8 +824,8 @@
       <c r="G2" t="s">
         <v>39</v>
       </c>
-      <c r="H2">
-        <v>560002</v>
+      <c r="H2" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="I2" t="s">
         <v>40</v>
@@ -827,11 +839,11 @@
       <c r="L2" t="s">
         <v>43</v>
       </c>
-      <c r="M2">
-        <v>8</v>
-      </c>
-      <c r="N2">
-        <v>14</v>
+      <c r="M2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="O2" t="s">
         <v>44</v>

</xml_diff>